<commit_message>
Adding some polish names of taxons to BazaPolskichRodzinWGore.xlsx
</commit_message>
<xml_diff>
--- a/BazaPolskichRodzinWGore.xlsx
+++ b/BazaPolskichRodzinWGore.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="574">
   <si>
     <t>Rodzina polska (13)</t>
   </si>
@@ -1644,6 +1644,108 @@
   </si>
   <si>
     <t>Ogórecznikowce</t>
+  </si>
+  <si>
+    <t>Paciorecznikowate</t>
+  </si>
+  <si>
+    <t>Zmienkowate</t>
+  </si>
+  <si>
+    <t>Przęstkowate</t>
+  </si>
+  <si>
+    <t>Wrońcowate</t>
+  </si>
+  <si>
+    <t>Orlicowate</t>
+  </si>
+  <si>
+    <t>Rzęsowate</t>
+  </si>
+  <si>
+    <t>Martyniowate</t>
+  </si>
+  <si>
+    <t>Korzeniówkowate</t>
+  </si>
+  <si>
+    <t>Jaśminowcowate</t>
+  </si>
+  <si>
+    <t>Bagnicowate</t>
+  </si>
+  <si>
+    <t>Grujecznikowce</t>
+  </si>
+  <si>
+    <t>Agrestowce</t>
+  </si>
+  <si>
+    <t>Męczennicowce</t>
+  </si>
+  <si>
+    <t>Wielosiłowe</t>
+  </si>
+  <si>
+    <t>Krzyżownicowce</t>
+  </si>
+  <si>
+    <t>Tamaryszkowce</t>
+  </si>
+  <si>
+    <t>Plantae</t>
+  </si>
+  <si>
+    <t>Rośliny</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widłakowe </t>
+  </si>
+  <si>
+    <t>Jednoliścienne</t>
+  </si>
+  <si>
+    <t>Cisowe</t>
+  </si>
+  <si>
+    <t>Miłorzębowe</t>
+  </si>
+  <si>
+    <t>Szpilkowe</t>
+  </si>
+  <si>
+    <t>Dwuliścienne</t>
+  </si>
+  <si>
+    <t>Widłaki różnozarodnikowe</t>
+  </si>
+  <si>
+    <t>Paprocie grubozarodniowe</t>
+  </si>
+  <si>
+    <t>Paprocie cienkozarodniowe</t>
+  </si>
+  <si>
+    <t>Widłaki jednakozarodnikowe</t>
+  </si>
+  <si>
+    <t>Skrzypowe</t>
+  </si>
+  <si>
+    <t>Paprociowe</t>
+  </si>
+  <si>
+    <t>Kotkowe</t>
+  </si>
+  <si>
+    <t>Astrowe</t>
+  </si>
+  <si>
+    <t>Śródłone</t>
+  </si>
+  <si>
+    <t>Ukęślowe</t>
   </si>
 </sst>
 </file>
@@ -1977,13 +2079,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P172"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.85546875"/>
+    <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="19"/>
     <col min="3" max="3" width="19.7109375"/>
     <col min="4" max="4" width="16.140625"/>
@@ -1991,7 +2093,7 @@
     <col min="6" max="6" width="19.28515625"/>
     <col min="7" max="7" width="18.5703125"/>
     <col min="8" max="8" width="19.85546875"/>
-    <col min="9" max="9" width="15.42578125"/>
+    <col min="9" max="9" width="26.85546875" customWidth="1"/>
     <col min="10" max="10" width="18.140625"/>
     <col min="11" max="11" width="22"/>
     <col min="12" max="12" width="23.140625"/>
@@ -2069,11 +2171,15 @@
       <c r="F2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="2"/>
+      <c r="G2" s="2" t="s">
+        <v>570</v>
+      </c>
       <c r="H2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="2"/>
+      <c r="I2" s="2" t="s">
+        <v>562</v>
+      </c>
       <c r="J2" s="2" t="s">
         <v>22</v>
       </c>
@@ -2089,8 +2195,12 @@
       <c r="N2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
+      <c r="O2" s="2" t="s">
+        <v>557</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>556</v>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -2109,11 +2219,15 @@
       <c r="F3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>571</v>
+      </c>
       <c r="H3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>563</v>
+      </c>
       <c r="J3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2149,15 +2263,21 @@
       <c r="F4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>572</v>
+      </c>
       <c r="H4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>565</v>
+      </c>
       <c r="J4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2" t="s">
+        <v>558</v>
+      </c>
       <c r="L4" s="2" t="s">
         <v>45</v>
       </c>
@@ -2183,15 +2303,21 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="2"/>
+      <c r="G5" s="2" t="s">
+        <v>573</v>
+      </c>
       <c r="H5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>561</v>
+      </c>
       <c r="J5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2" t="s">
+        <v>569</v>
+      </c>
       <c r="L5" s="2" t="s">
         <v>53</v>
       </c>
@@ -2220,11 +2346,15 @@
       <c r="H6" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="I6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>564</v>
+      </c>
       <c r="J6" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2" t="s">
+        <v>568</v>
+      </c>
       <c r="L6" s="2" t="s">
         <v>61</v>
       </c>
@@ -2253,7 +2383,9 @@
       <c r="H7" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>566</v>
+      </c>
       <c r="J7" s="2" t="s">
         <v>68</v>
       </c>
@@ -2283,7 +2415,9 @@
       <c r="H8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="I8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>567</v>
+      </c>
       <c r="J8" s="2" t="s">
         <v>74</v>
       </c>
@@ -2313,7 +2447,9 @@
       <c r="H9" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>559</v>
+      </c>
       <c r="J9" s="2" t="s">
         <v>80</v>
       </c>
@@ -2343,7 +2479,9 @@
       <c r="H10" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>568</v>
+      </c>
       <c r="J10" s="2" t="s">
         <v>87</v>
       </c>
@@ -2373,7 +2511,9 @@
       <c r="H11" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="I11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>560</v>
+      </c>
       <c r="J11" s="2" t="s">
         <v>94</v>
       </c>
@@ -2439,7 +2579,9 @@
       <c r="B14" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="2" t="s">
+        <v>550</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>107</v>
       </c>
@@ -2710,7 +2852,9 @@
       <c r="B27" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C27" s="2"/>
+      <c r="C27" s="2" t="s">
+        <v>551</v>
+      </c>
       <c r="D27" s="2" t="s">
         <v>155</v>
       </c>
@@ -2954,7 +3098,9 @@
       <c r="P38" s="2"/>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A39" s="2"/>
+      <c r="A39" s="2" t="s">
+        <v>540</v>
+      </c>
       <c r="B39" s="2" t="s">
         <v>188</v>
       </c>
@@ -3231,7 +3377,9 @@
       <c r="B52" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C52" s="2"/>
+      <c r="C52" s="2" t="s">
+        <v>552</v>
+      </c>
       <c r="D52" s="2" t="s">
         <v>228</v>
       </c>
@@ -3244,7 +3392,9 @@
       <c r="P52" s="2"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A53" s="2"/>
+      <c r="A53" s="2" t="s">
+        <v>541</v>
+      </c>
       <c r="B53" s="2" t="s">
         <v>229</v>
       </c>
@@ -3332,7 +3482,9 @@
       <c r="B57" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="C57" s="2"/>
+      <c r="C57" s="2" t="s">
+        <v>553</v>
+      </c>
       <c r="D57" s="2" t="s">
         <v>242</v>
       </c>
@@ -3351,7 +3503,9 @@
       <c r="B58" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C58" s="2"/>
+      <c r="C58" s="2" t="s">
+        <v>554</v>
+      </c>
       <c r="D58" s="2" t="s">
         <v>245</v>
       </c>
@@ -3706,7 +3860,9 @@
       <c r="B75" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C75" s="2"/>
+      <c r="C75" s="2" t="s">
+        <v>555</v>
+      </c>
       <c r="D75" s="2" t="s">
         <v>295</v>
       </c>
@@ -3719,7 +3875,9 @@
       <c r="P75" s="2"/>
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A76" s="2"/>
+      <c r="A76" s="2" t="s">
+        <v>542</v>
+      </c>
       <c r="B76" s="2" t="s">
         <v>296</v>
       </c>
@@ -3738,7 +3896,9 @@
       <c r="P76" s="2"/>
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A77" s="2"/>
+      <c r="A77" s="2" t="s">
+        <v>543</v>
+      </c>
       <c r="B77" s="2" t="s">
         <v>298</v>
       </c>
@@ -3857,7 +4017,9 @@
       <c r="P82" s="2"/>
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A83" s="2"/>
+      <c r="A83" s="2" t="s">
+        <v>544</v>
+      </c>
       <c r="B83" s="2" t="s">
         <v>316</v>
       </c>
@@ -3967,7 +4129,9 @@
       <c r="P89" s="2"/>
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A90" s="2"/>
+      <c r="A90" s="2" t="s">
+        <v>545</v>
+      </c>
       <c r="B90" s="2" t="s">
         <v>329</v>
       </c>
@@ -4141,7 +4305,9 @@
       <c r="P100" s="2"/>
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A101" s="2"/>
+      <c r="A101" s="2" t="s">
+        <v>546</v>
+      </c>
       <c r="B101" s="2" t="s">
         <v>350</v>
       </c>
@@ -4171,7 +4337,9 @@
       <c r="P102" s="2"/>
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A103" s="2"/>
+      <c r="A103" s="2" t="s">
+        <v>547</v>
+      </c>
       <c r="B103" s="2" t="s">
         <v>353</v>
       </c>
@@ -4425,7 +4593,9 @@
       <c r="P118" s="2"/>
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A119" s="2"/>
+      <c r="A119" s="2" t="s">
+        <v>548</v>
+      </c>
       <c r="B119" s="2" t="s">
         <v>384</v>
       </c>
@@ -4871,7 +5041,9 @@
       <c r="P146" s="2"/>
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
+      <c r="A147" s="2" t="s">
+        <v>549</v>
+      </c>
       <c r="B147" s="2" t="s">
         <v>439</v>
       </c>

</xml_diff>

<commit_message>
New records in BazaPolskichRodzinWGore.xlsx
</commit_message>
<xml_diff>
--- a/BazaPolskichRodzinWGore.xlsx
+++ b/BazaPolskichRodzinWGore.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafal\Desktop\botanikaTesty\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rafal\Desktop\botanikaTesty\Nowy folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="580">
   <si>
     <t>Rodzina polska (13)</t>
   </si>
@@ -1746,6 +1746,24 @@
   </si>
   <si>
     <t>Ukęślowe</t>
+  </si>
+  <si>
+    <t>Bagienne</t>
+  </si>
+  <si>
+    <t>Sitowe</t>
+  </si>
+  <si>
+    <t>Liliokwiatowe</t>
+  </si>
+  <si>
+    <t>Wieloowockowe</t>
+  </si>
+  <si>
+    <t>Różowe</t>
+  </si>
+  <si>
+    <t>Kolbokwiatowe</t>
   </si>
 </sst>
 </file>
@@ -2080,7 +2098,7 @@
   <dimension ref="A1:P172"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2379,7 +2397,9 @@
       <c r="F7" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="G7" s="2"/>
+      <c r="G7" s="2" t="s">
+        <v>574</v>
+      </c>
       <c r="H7" s="2" t="s">
         <v>67</v>
       </c>
@@ -2411,7 +2431,9 @@
       <c r="F8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G8" s="2"/>
+      <c r="G8" s="2" t="s">
+        <v>575</v>
+      </c>
       <c r="H8" s="2" t="s">
         <v>73</v>
       </c>
@@ -2443,7 +2465,9 @@
       <c r="F9" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>576</v>
+      </c>
       <c r="H9" s="2" t="s">
         <v>79</v>
       </c>
@@ -2475,7 +2499,9 @@
       <c r="F10" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>577</v>
+      </c>
       <c r="H10" s="2" t="s">
         <v>86</v>
       </c>
@@ -2507,7 +2533,9 @@
       <c r="F11" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>578</v>
+      </c>
       <c r="H11" s="2" t="s">
         <v>93</v>
       </c>
@@ -2539,7 +2567,9 @@
       <c r="F12" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>579</v>
+      </c>
       <c r="H12" s="2" t="s">
         <v>100</v>
       </c>

</xml_diff>